<commit_message>
Included wave 16, added HWLE calculations
</commit_message>
<xml_diff>
--- a/Results/quality.xlsx
+++ b/Results/quality.xlsx
@@ -471,52 +471,52 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.6835195325241248</v>
+        <v>0.674938964098174</v>
       </c>
       <c r="E2">
-        <v>0.4165451963211997</v>
+        <v>0.4261704314606063</v>
       </c>
       <c r="F2">
-        <v>0.1718435557107438</v>
+        <v>0.180826786245351</v>
       </c>
       <c r="G2">
-        <v>0.8175230068533549</v>
+        <v>0.8230139591873777</v>
       </c>
       <c r="H2">
-        <v>1.044098255695232</v>
+        <v>1.041926982080775</v>
       </c>
       <c r="I2">
-        <v>1.237123360808975</v>
+        <v>1.233865740654225</v>
       </c>
       <c r="J2">
-        <v>1.050483634589852</v>
+        <v>1.097992935039133</v>
       </c>
       <c r="K2">
-        <v>1.053956506267101</v>
+        <v>1.05454966485305</v>
       </c>
       <c r="L2">
-        <v>1.013214108030252</v>
+        <v>1.010707186697167</v>
       </c>
       <c r="M2">
-        <v>1.177261567584297</v>
+        <v>1.174665098728651</v>
       </c>
       <c r="N2">
-        <v>0.9393582234967901</v>
+        <v>0.9915038189280895</v>
       </c>
       <c r="O2">
-        <v>1.032635334999701</v>
+        <v>1.032568395975954</v>
       </c>
       <c r="P2">
-        <v>1.080641699909626</v>
+        <v>1.073564370337879</v>
       </c>
       <c r="Q2">
-        <v>1.308272987123011</v>
+        <v>1.29634843634297</v>
       </c>
       <c r="R2">
-        <v>1.177921432600948</v>
+        <v>1.222957310708584</v>
       </c>
       <c r="S2">
-        <v>1.080691074729922</v>
+        <v>1.077218693888152</v>
       </c>
     </row>
     <row r="3">
@@ -536,52 +536,52 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.6577170628572603</v>
+        <v>0.6441171104461911</v>
       </c>
       <c r="E3">
-        <v>0.4944469305432463</v>
+        <v>0.4896700135395199</v>
       </c>
       <c r="F3">
-        <v>0.2040440544126476</v>
+        <v>0.2134211924131378</v>
       </c>
       <c r="G3">
-        <v>0.8386909240581151</v>
+        <v>0.8341483890899861</v>
       </c>
       <c r="H3">
-        <v>1.054004392494821</v>
+        <v>1.055465555685529</v>
       </c>
       <c r="I3">
-        <v>1.193829524087098</v>
+        <v>1.195516700226279</v>
       </c>
       <c r="J3">
-        <v>1.106747649520144</v>
+        <v>1.133158779166932</v>
       </c>
       <c r="K3">
-        <v>1.05346833756508</v>
+        <v>1.056043184458593</v>
       </c>
       <c r="L3">
-        <v>1.021972262622803</v>
+        <v>1.023704670438494</v>
       </c>
       <c r="M3">
-        <v>1.146143366440801</v>
+        <v>1.145122786467195</v>
       </c>
       <c r="N3">
-        <v>1.0015820107145</v>
+        <v>1.032607704228432</v>
       </c>
       <c r="O3">
-        <v>1.035052565250807</v>
+        <v>1.036617911138447</v>
       </c>
       <c r="P3">
-        <v>1.090851643787171</v>
+        <v>1.08991916321945</v>
       </c>
       <c r="Q3">
-        <v>1.250298774655401</v>
+        <v>1.256181930348764</v>
       </c>
       <c r="R3">
-        <v>1.214972318295113</v>
+        <v>1.253723894334721</v>
       </c>
       <c r="S3">
-        <v>1.077299313986833</v>
+        <v>1.079945567570936</v>
       </c>
     </row>
     <row r="4">
@@ -601,52 +601,52 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.581003380315646</v>
+        <v>0.5793104818050514</v>
       </c>
       <c r="E4">
-        <v>0.4799401324888191</v>
+        <v>0.4867226343139558</v>
       </c>
       <c r="F4">
-        <v>0.2523767916092918</v>
+        <v>0.2566708241273308</v>
       </c>
       <c r="G4">
-        <v>0.8193264327177946</v>
+        <v>0.8204014402300149</v>
       </c>
       <c r="H4">
-        <v>1.058382813377533</v>
+        <v>1.054261323083509</v>
       </c>
       <c r="I4">
-        <v>1.211358862466423</v>
+        <v>1.209187532097304</v>
       </c>
       <c r="J4">
-        <v>1.045574404598978</v>
+        <v>1.088920153175076</v>
       </c>
       <c r="K4">
-        <v>1.05342325241806</v>
+        <v>1.055354881088704</v>
       </c>
       <c r="L4">
-        <v>1.016730250379123</v>
+        <v>1.013937967541522</v>
       </c>
       <c r="M4">
-        <v>1.158456093903216</v>
+        <v>1.155656083360111</v>
       </c>
       <c r="N4">
-        <v>0.9450488182099978</v>
+        <v>0.9920283517487014</v>
       </c>
       <c r="O4">
-        <v>1.032529503223918</v>
+        <v>1.034558679712147</v>
       </c>
       <c r="P4">
-        <v>1.103426121425787</v>
+        <v>1.095240732127239</v>
       </c>
       <c r="Q4">
-        <v>1.272277271588753</v>
+        <v>1.266284659087497</v>
       </c>
       <c r="R4">
-        <v>1.158013837665733</v>
+        <v>1.200932662416647</v>
       </c>
       <c r="S4">
-        <v>1.076964136236134</v>
+        <v>1.077087706667803</v>
       </c>
     </row>
     <row r="5">
@@ -666,52 +666,52 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.5616648626101857</v>
+        <v>0.5536919398332348</v>
       </c>
       <c r="E5">
-        <v>0.4939650699472856</v>
+        <v>0.4884483000010756</v>
       </c>
       <c r="F5">
-        <v>0.263178312295711</v>
+        <v>0.2710922582746357</v>
       </c>
       <c r="G5">
-        <v>0.8369997955036165</v>
+        <v>0.8293742171902622</v>
       </c>
       <c r="H5">
-        <v>1.069159225410057</v>
+        <v>1.069558625296981</v>
       </c>
       <c r="I5">
-        <v>1.19401426989448</v>
+        <v>1.195984760904655</v>
       </c>
       <c r="J5">
-        <v>1.098817005782724</v>
+        <v>1.123395728536402</v>
       </c>
       <c r="K5">
-        <v>1.054028887750431</v>
+        <v>1.057656432559984</v>
       </c>
       <c r="L5">
-        <v>1.027933323073099</v>
+        <v>1.030283208296995</v>
       </c>
       <c r="M5">
-        <v>1.146196841934884</v>
+        <v>1.146036960518357</v>
       </c>
       <c r="N5">
-        <v>1.001467766537552</v>
+        <v>1.029565199518718</v>
       </c>
       <c r="O5">
-        <v>1.036108510667731</v>
+        <v>1.040508158031597</v>
       </c>
       <c r="P5">
-        <v>1.112353739243522</v>
+        <v>1.113419186938668</v>
       </c>
       <c r="Q5">
-        <v>1.249971289715862</v>
+        <v>1.249263133608853</v>
       </c>
       <c r="R5">
-        <v>1.201077429356429</v>
+        <v>1.232708510846813</v>
       </c>
       <c r="S5">
-        <v>1.074023842891252</v>
+        <v>1.07872705680802</v>
       </c>
     </row>
     <row r="6">
@@ -731,52 +731,52 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.5664552206316302</v>
+        <v>0.5673294387761182</v>
       </c>
       <c r="E6">
-        <v>0.6032116331986909</v>
+        <v>0.6076510503033095</v>
       </c>
       <c r="F6">
-        <v>0.06587955580206835</v>
+        <v>0.06636307852937416</v>
       </c>
       <c r="G6">
-        <v>0.8268440813116509</v>
+        <v>0.8285866013349112</v>
       </c>
       <c r="H6">
-        <v>1.060409947850499</v>
+        <v>1.055806660484498</v>
       </c>
       <c r="I6">
-        <v>1.161259776203038</v>
+        <v>1.159902840052803</v>
       </c>
       <c r="J6">
-        <v>1.056943099933577</v>
+        <v>1.111685563760645</v>
       </c>
       <c r="K6">
-        <v>1.051200363677547</v>
+        <v>1.052832095715404</v>
       </c>
       <c r="L6">
-        <v>1.017066322711784</v>
+        <v>1.013676351923526</v>
       </c>
       <c r="M6">
-        <v>1.117767919908355</v>
+        <v>1.119272686005423</v>
       </c>
       <c r="N6">
-        <v>0.9305699109706342</v>
+        <v>0.9902224193208965</v>
       </c>
       <c r="O6">
-        <v>1.031149756242346</v>
+        <v>1.032200461878069</v>
       </c>
       <c r="P6">
-        <v>1.107693991981422</v>
+        <v>1.098418896908027</v>
       </c>
       <c r="Q6">
-        <v>1.207719926536266</v>
+        <v>1.207786637198979</v>
       </c>
       <c r="R6">
-        <v>1.207015715922681</v>
+        <v>1.257142300420107</v>
       </c>
       <c r="S6">
-        <v>1.075558763509092</v>
+        <v>1.075008478551248</v>
       </c>
     </row>
     <row r="7">
@@ -796,52 +796,52 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.5381907038819844</v>
+        <v>0.5321746027977414</v>
       </c>
       <c r="E7">
-        <v>0.6424496733481566</v>
+        <v>0.6389400510944171</v>
       </c>
       <c r="F7">
-        <v>0.08519436753152562</v>
+        <v>0.08671628640832378</v>
       </c>
       <c r="G7">
-        <v>0.8398475075689038</v>
+        <v>0.8356756939797073</v>
       </c>
       <c r="H7">
-        <v>1.072862908953344</v>
+        <v>1.072912175272488</v>
       </c>
       <c r="I7">
-        <v>1.137085132776632</v>
+        <v>1.1383286337601</v>
       </c>
       <c r="J7">
-        <v>1.122686879311817</v>
+        <v>1.154608467914363</v>
       </c>
       <c r="K7">
-        <v>1.053084970434521</v>
+        <v>1.055527090408077</v>
       </c>
       <c r="L7">
-        <v>1.029044207173212</v>
+        <v>1.0318548727902</v>
       </c>
       <c r="M7">
-        <v>1.102392628159572</v>
+        <v>1.102291510531117</v>
       </c>
       <c r="N7">
-        <v>1.001829012983137</v>
+        <v>1.037159841472909</v>
       </c>
       <c r="O7">
-        <v>1.035097045268287</v>
+        <v>1.037785052968744</v>
       </c>
       <c r="P7">
-        <v>1.120741644427255</v>
+        <v>1.118544264009534</v>
       </c>
       <c r="Q7">
-        <v>1.177113732523665</v>
+        <v>1.177950555766082</v>
       </c>
       <c r="R7">
-        <v>1.25171213644987</v>
+        <v>1.290960085999444</v>
       </c>
       <c r="S7">
-        <v>1.075633723840007</v>
+        <v>1.075640470881273</v>
       </c>
     </row>
     <row r="8">
@@ -861,52 +861,52 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.5370719745165503</v>
+        <v>0.5366745109956695</v>
       </c>
       <c r="E8">
-        <v>0.5030314883448698</v>
+        <v>0.5065669743504568</v>
       </c>
       <c r="F8">
-        <v>0.07906600862062732</v>
+        <v>0.08608381246519096</v>
       </c>
       <c r="G8">
-        <v>0.7686456608164728</v>
+        <v>0.7744302918274106</v>
       </c>
       <c r="H8">
-        <v>1.064504197049108</v>
+        <v>1.059760590564652</v>
       </c>
       <c r="I8">
-        <v>1.201974245403202</v>
+        <v>1.201099919442132</v>
       </c>
       <c r="J8">
-        <v>1.056139266225322</v>
+        <v>1.109326486868178</v>
       </c>
       <c r="K8">
-        <v>1.068409017689398</v>
+        <v>1.069523855809862</v>
       </c>
       <c r="L8">
-        <v>1.019350671261173</v>
+        <v>1.015161159035475</v>
       </c>
       <c r="M8">
-        <v>1.150516758427119</v>
+        <v>1.150433591300263</v>
       </c>
       <c r="N8">
-        <v>0.9320771727041821</v>
+        <v>0.990336500880593</v>
       </c>
       <c r="O8">
-        <v>1.043327013531331</v>
+        <v>1.043403951791956</v>
       </c>
       <c r="P8">
-        <v>1.110405551463595</v>
+        <v>1.107401539299718</v>
       </c>
       <c r="Q8">
-        <v>1.260815716801262</v>
+        <v>1.252835500190896</v>
       </c>
       <c r="R8">
-        <v>1.20311753225668</v>
+        <v>1.250998030696123</v>
       </c>
       <c r="S8">
-        <v>1.09744546864995</v>
+        <v>1.096237460115484</v>
       </c>
     </row>
     <row r="9">
@@ -926,52 +926,52 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.4503148404208295</v>
+        <v>0.4502154638456338</v>
       </c>
       <c r="E9">
-        <v>0.5572388255215259</v>
+        <v>0.556076520392226</v>
       </c>
       <c r="F9">
-        <v>0.1013268383487709</v>
+        <v>0.1059236198199832</v>
       </c>
       <c r="G9">
-        <v>0.7679803848535932</v>
+        <v>0.7686914758147056</v>
       </c>
       <c r="H9">
-        <v>1.086727703560965</v>
+        <v>1.085685785128206</v>
       </c>
       <c r="I9">
-        <v>1.169755052274979</v>
+        <v>1.170075159580303</v>
       </c>
       <c r="J9">
-        <v>1.120523313161906</v>
+        <v>1.151356886453636</v>
       </c>
       <c r="K9">
-        <v>1.076906417273369</v>
+        <v>1.07816183524919</v>
       </c>
       <c r="L9">
-        <v>1.035001138198733</v>
+        <v>1.036671976484882</v>
       </c>
       <c r="M9">
-        <v>1.129628157823973</v>
+        <v>1.126542437134207</v>
       </c>
       <c r="N9">
-        <v>1.001784824149812</v>
+        <v>1.036041202895931</v>
       </c>
       <c r="O9">
-        <v>1.051708400033905</v>
+        <v>1.055375549022575</v>
       </c>
       <c r="P9">
-        <v>1.143951573749473</v>
+        <v>1.137885000684985</v>
       </c>
       <c r="Q9">
-        <v>1.218419535632835</v>
+        <v>1.215122584012405</v>
       </c>
       <c r="R9">
-        <v>1.245031906178167</v>
+        <v>1.283668811130095</v>
       </c>
       <c r="S9">
-        <v>1.103342044859157</v>
+        <v>1.105249064198194</v>
       </c>
     </row>
     <row r="10">
@@ -991,52 +991,52 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.4664148047722854</v>
+        <v>0.4702501327887972</v>
       </c>
       <c r="E10">
-        <v>0.5642088886363581</v>
+        <v>0.5632956988270298</v>
       </c>
       <c r="F10">
-        <v>0.1072299077005703</v>
+        <v>0.1155076254646437</v>
       </c>
       <c r="G10">
-        <v>0.7784494204094269</v>
+        <v>0.7819745765695939</v>
       </c>
       <c r="H10">
-        <v>1.074349537467539</v>
+        <v>1.068328131448411</v>
       </c>
       <c r="I10">
-        <v>1.177110981494486</v>
+        <v>1.177979979492275</v>
       </c>
       <c r="J10">
-        <v>1.05442242154026</v>
+        <v>1.105806686968175</v>
       </c>
       <c r="K10">
-        <v>1.065510150238786</v>
+        <v>1.067198597827071</v>
       </c>
       <c r="L10">
-        <v>1.021298947293009</v>
+        <v>1.017059624007728</v>
       </c>
       <c r="M10">
-        <v>1.132783373620724</v>
+        <v>1.133422692002327</v>
       </c>
       <c r="N10">
-        <v>0.9341703872701977</v>
+        <v>0.990581358706739</v>
       </c>
       <c r="O10">
-        <v>1.042270096761871</v>
+        <v>1.041845189435226</v>
       </c>
       <c r="P10">
-        <v>1.130754085254148</v>
+        <v>1.12178660647591</v>
       </c>
       <c r="Q10">
-        <v>1.229568451598431</v>
+        <v>1.228293256946802</v>
       </c>
       <c r="R10">
-        <v>1.196362850826908</v>
+        <v>1.242135751984562</v>
       </c>
       <c r="S10">
-        <v>1.092956980082138</v>
+        <v>1.093401693712098</v>
       </c>
     </row>
     <row r="11">
@@ -1056,52 +1056,52 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.3906411003626096</v>
+        <v>0.3934301481375332</v>
       </c>
       <c r="E11">
-        <v>0.554157123742281</v>
+        <v>0.5508912505743382</v>
       </c>
       <c r="F11">
-        <v>0.1190177831141052</v>
+        <v>0.1258229794731973</v>
       </c>
       <c r="G11">
-        <v>0.7735265738580027</v>
+        <v>0.7735319205615088</v>
       </c>
       <c r="H11">
-        <v>1.096142850300793</v>
+        <v>1.094535969228029</v>
       </c>
       <c r="I11">
-        <v>1.170936579646361</v>
+        <v>1.172061730762623</v>
       </c>
       <c r="J11">
-        <v>1.118150736159423</v>
+        <v>1.14798815287975</v>
       </c>
       <c r="K11">
-        <v>1.075068048885502</v>
+        <v>1.076526192783505</v>
       </c>
       <c r="L11">
-        <v>1.038417612170542</v>
+        <v>1.04057283796357</v>
       </c>
       <c r="M11">
-        <v>1.128334827182179</v>
+        <v>1.12838796518489</v>
       </c>
       <c r="N11">
-        <v>1.001744630190954</v>
+        <v>1.035643677792577</v>
       </c>
       <c r="O11">
-        <v>1.051408116696234</v>
+        <v>1.054727696723921</v>
       </c>
       <c r="P11">
-        <v>1.156090774583735</v>
+        <v>1.153929128012093</v>
       </c>
       <c r="Q11">
-        <v>1.223374416771505</v>
+        <v>1.217549395141203</v>
       </c>
       <c r="R11">
-        <v>1.240218270360443</v>
+        <v>1.280055421069166</v>
       </c>
       <c r="S11">
-        <v>1.10412702004948</v>
+        <v>1.102352208888455</v>
       </c>
     </row>
     <row r="12">
@@ -1121,52 +1121,52 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.4106076906461978</v>
+        <v>0.4102269369216154</v>
       </c>
       <c r="E12">
-        <v>0.6348649022978572</v>
+        <v>0.6341206903601967</v>
       </c>
       <c r="F12">
-        <v>0.02291004468227386</v>
+        <v>0.02458487439929756</v>
       </c>
       <c r="G12">
-        <v>0.7782213785350327</v>
+        <v>0.7794388229132639</v>
       </c>
       <c r="H12">
-        <v>1.082125677360067</v>
+        <v>1.076070035828222</v>
       </c>
       <c r="I12">
-        <v>1.148395490054291</v>
+        <v>1.149115069055726</v>
       </c>
       <c r="J12">
-        <v>1.05956248074361</v>
+        <v>1.116683247735937</v>
       </c>
       <c r="K12">
-        <v>1.065577579795864</v>
+        <v>1.067980153883513</v>
       </c>
       <c r="L12">
-        <v>1.023281762176376</v>
+        <v>1.01954566634613</v>
       </c>
       <c r="M12">
-        <v>1.11136246562521</v>
+        <v>1.112586325036329</v>
       </c>
       <c r="N12">
-        <v>0.9279531562222474</v>
+        <v>0.9897633307988506</v>
       </c>
       <c r="O12">
-        <v>1.041697088410233</v>
+        <v>1.042611948531186</v>
       </c>
       <c r="P12">
-        <v>1.143563474572525</v>
+        <v>1.137597597004142</v>
       </c>
       <c r="Q12">
-        <v>1.192031752212329</v>
+        <v>1.18832785078368</v>
       </c>
       <c r="R12">
-        <v>1.216672860596275</v>
+        <v>1.266852036480633</v>
       </c>
       <c r="S12">
-        <v>1.092734432266782</v>
+        <v>1.093421461787918</v>
       </c>
     </row>
     <row r="13">
@@ -1186,52 +1186,52 @@
         </is>
       </c>
       <c r="D13">
-        <v>0.3302845308079958</v>
+        <v>0.3285951053771827</v>
       </c>
       <c r="E13">
-        <v>0.6509847487881099</v>
+        <v>0.6515978742458469</v>
       </c>
       <c r="F13">
-        <v>0.03186464572458923</v>
+        <v>0.03330498393649274</v>
       </c>
       <c r="G13">
-        <v>0.7678835954183992</v>
+        <v>0.7689119920065082</v>
       </c>
       <c r="H13">
-        <v>1.105665731865027</v>
+        <v>1.104640730598003</v>
       </c>
       <c r="I13">
-        <v>1.133812776795585</v>
+        <v>1.133479191477118</v>
       </c>
       <c r="J13">
-        <v>1.129839062148083</v>
+        <v>1.163650389413219</v>
       </c>
       <c r="K13">
-        <v>1.076938499598331</v>
+        <v>1.078087320268326</v>
       </c>
       <c r="L13">
-        <v>1.04320478350242</v>
+        <v>1.045497389127326</v>
       </c>
       <c r="M13">
-        <v>1.102747176908807</v>
+        <v>1.100012818353924</v>
       </c>
       <c r="N13">
-        <v>1.001918740400947</v>
+        <v>1.039206406359893</v>
       </c>
       <c r="O13">
-        <v>1.053282848891016</v>
+        <v>1.055443225620529</v>
       </c>
       <c r="P13">
-        <v>1.173172326714252</v>
+        <v>1.171485320654107</v>
       </c>
       <c r="Q13">
-        <v>1.170634527022718</v>
+        <v>1.166936724304705</v>
       </c>
       <c r="R13">
-        <v>1.263791016657192</v>
+        <v>1.307716257265322</v>
       </c>
       <c r="S13">
-        <v>1.103020414838134</v>
+        <v>1.102622378347218</v>
       </c>
     </row>
     <row r="14">
@@ -1251,52 +1251,52 @@
         </is>
       </c>
       <c r="D14">
-        <v>0.2084242391305729</v>
+        <v>0.2056467488344851</v>
       </c>
       <c r="E14">
-        <v>0.6170291554785711</v>
+        <v>0.6150382505849697</v>
       </c>
       <c r="F14">
-        <v>0.03060720672784347</v>
+        <v>0.03248642585510493</v>
       </c>
       <c r="G14">
-        <v>0.705501664307754</v>
+        <v>0.7038970011909848</v>
       </c>
       <c r="H14">
-        <v>1.110297834755405</v>
+        <v>1.102457172189288</v>
       </c>
       <c r="I14">
-        <v>1.155644161590905</v>
+        <v>1.1568921672678</v>
       </c>
       <c r="J14">
-        <v>1.059093269015841</v>
+        <v>1.11573803101557</v>
       </c>
       <c r="K14">
-        <v>1.08708002593324</v>
+        <v>1.09126323902638</v>
       </c>
       <c r="L14">
-        <v>1.032028395153306</v>
+        <v>1.025394808612565</v>
       </c>
       <c r="M14">
-        <v>1.116487137873932</v>
+        <v>1.117991994497274</v>
       </c>
       <c r="N14">
-        <v>0.9286757853284469</v>
+        <v>0.9899215151459679</v>
       </c>
       <c r="O14">
-        <v>1.055772744729348</v>
+        <v>1.060060603778776</v>
       </c>
       <c r="P14">
-        <v>1.194189475733554</v>
+        <v>1.184216722729051</v>
       </c>
       <c r="Q14">
-        <v>1.203620956084896</v>
+        <v>1.200482585034327</v>
       </c>
       <c r="R14">
-        <v>1.214669099716139</v>
+        <v>1.266381556183599</v>
       </c>
       <c r="S14">
-        <v>1.124642813695595</v>
+        <v>1.126734206627765</v>
       </c>
     </row>
     <row r="15">
@@ -1316,52 +1316,52 @@
         </is>
       </c>
       <c r="D15">
-        <v>0.2363596193216282</v>
+        <v>0.2336029685724909</v>
       </c>
       <c r="E15">
-        <v>0.6768238920349368</v>
+        <v>0.6727178804232677</v>
       </c>
       <c r="F15">
-        <v>0.0310812684235801</v>
+        <v>0.0305489784264249</v>
       </c>
       <c r="G15">
-        <v>0.7392574504319697</v>
+        <v>0.7344736847637986</v>
       </c>
       <c r="H15">
-        <v>1.120484927432569</v>
+        <v>1.119445577384072</v>
       </c>
       <c r="I15">
-        <v>1.12390602488182</v>
+        <v>1.12538773295788</v>
       </c>
       <c r="J15">
-        <v>1.12994412284401</v>
+        <v>1.164116949566578</v>
       </c>
       <c r="K15">
-        <v>1.086427069130977</v>
+        <v>1.089724424030267</v>
       </c>
       <c r="L15">
-        <v>1.049752996338377</v>
+        <v>1.051841723456482</v>
       </c>
       <c r="M15">
-        <v>1.092596943074343</v>
+        <v>1.094356349189918</v>
       </c>
       <c r="N15">
-        <v>1.001921930265669</v>
+        <v>1.039164607376752</v>
       </c>
       <c r="O15">
-        <v>1.058579656712467</v>
+        <v>1.063599317778712</v>
       </c>
       <c r="P15">
-        <v>1.199021002126987</v>
+        <v>1.191496590273751</v>
       </c>
       <c r="Q15">
-        <v>1.161494096996591</v>
+        <v>1.159732103398967</v>
       </c>
       <c r="R15">
-        <v>1.262459936810329</v>
+        <v>1.309261531899949</v>
       </c>
       <c r="S15">
-        <v>1.11816940764967</v>
+        <v>1.121132922998034</v>
       </c>
     </row>
     <row r="16">
@@ -1381,52 +1381,52 @@
         </is>
       </c>
       <c r="D16">
-        <v>0.2847340058688702</v>
+        <v>0.2727914238288439</v>
       </c>
       <c r="E16">
-        <v>0.63452696192628</v>
+        <v>0.6403956314770581</v>
       </c>
       <c r="F16">
-        <v>0.07488491118805768</v>
+        <v>0.0747512823137261</v>
       </c>
       <c r="G16">
-        <v>0.7491129596126874</v>
+        <v>0.7512854004693271</v>
       </c>
       <c r="H16">
-        <v>1.099664863840935</v>
+        <v>1.093796726074921</v>
       </c>
       <c r="I16">
-        <v>1.148532833266064</v>
+        <v>1.146557700400793</v>
       </c>
       <c r="J16">
-        <v>1.05639414197546</v>
+        <v>1.110682131647957</v>
       </c>
       <c r="K16">
-        <v>1.074184629708982</v>
+        <v>1.076657447028959</v>
       </c>
       <c r="L16">
-        <v>1.027238502104199</v>
+        <v>1.023374238972219</v>
       </c>
       <c r="M16">
-        <v>1.109570089706756</v>
+        <v>1.10800846558575</v>
       </c>
       <c r="N16">
-        <v>0.9323585693685164</v>
+        <v>0.9901845803956173</v>
       </c>
       <c r="O16">
-        <v>1.045488445675182</v>
+        <v>1.048342857589417</v>
       </c>
       <c r="P16">
-        <v>1.176537087374862</v>
+        <v>1.166761000655648</v>
       </c>
       <c r="Q16">
-        <v>1.197868008031604</v>
+        <v>1.191849504539064</v>
       </c>
       <c r="R16">
-        <v>1.199512780459306</v>
+        <v>1.252316234787269</v>
       </c>
       <c r="S16">
-        <v>1.110147578992588</v>
+        <v>1.11171744693004</v>
       </c>
     </row>
     <row r="17">
@@ -1446,52 +1446,52 @@
         </is>
       </c>
       <c r="D17">
-        <v>0.3270611757427432</v>
+        <v>0.3134091833571247</v>
       </c>
       <c r="E17">
-        <v>0.6353704724465569</v>
+        <v>0.6410177905508562</v>
       </c>
       <c r="F17">
-        <v>0.06580099135715321</v>
+        <v>0.06230039339440884</v>
       </c>
       <c r="G17">
-        <v>0.7751774536136742</v>
+        <v>0.7756873358210327</v>
       </c>
       <c r="H17">
-        <v>1.106174303322158</v>
+        <v>1.107007508063745</v>
       </c>
       <c r="I17">
-        <v>1.139799305085285</v>
+        <v>1.137532613982249</v>
       </c>
       <c r="J17">
-        <v>1.125287773663258</v>
+        <v>1.158741798833837</v>
       </c>
       <c r="K17">
-        <v>1.074520839774421</v>
+        <v>1.075797852948206</v>
       </c>
       <c r="L17">
-        <v>1.044191218642741</v>
+        <v>1.045577035929444</v>
       </c>
       <c r="M17">
-        <v>1.10149487311788</v>
+        <v>1.102182699320616</v>
       </c>
       <c r="N17">
-        <v>1.001861028740489</v>
+        <v>1.037895381079588</v>
       </c>
       <c r="O17">
-        <v>1.048967267030918</v>
+        <v>1.052242220500549</v>
       </c>
       <c r="P17">
-        <v>1.175625242699108</v>
+        <v>1.172834550246524</v>
       </c>
       <c r="Q17">
-        <v>1.186480890678051</v>
+        <v>1.178973051921884</v>
       </c>
       <c r="R17">
-        <v>1.255158002195386</v>
+        <v>1.300091878485186</v>
       </c>
       <c r="S17">
-        <v>1.110336569341654</v>
+        <v>1.109267182709991</v>
       </c>
     </row>
     <row r="18">
@@ -1511,52 +1511,52 @@
         </is>
       </c>
       <c r="D18">
-        <v>0.1514204882668275</v>
+        <v>0.1509077165077166</v>
       </c>
       <c r="E18">
-        <v>0.7121096388778528</v>
+        <v>0.7097457974267267</v>
       </c>
       <c r="F18">
-        <v>0.008228927771815584</v>
+        <v>0.0087839249075748</v>
       </c>
       <c r="G18">
-        <v>0.7507024640566946</v>
+        <v>0.74860038294492</v>
       </c>
       <c r="H18">
-        <v>1.118240713509426</v>
+        <v>1.109517515244912</v>
       </c>
       <c r="I18">
-        <v>1.117002258861124</v>
+        <v>1.118293858986007</v>
       </c>
       <c r="J18">
-        <v>1.060457427763088</v>
+        <v>1.118573423575552</v>
       </c>
       <c r="K18">
-        <v>1.073714630148952</v>
+        <v>1.077485008374524</v>
       </c>
       <c r="L18">
-        <v>1.033145783033963</v>
+        <v>1.027424867608665</v>
       </c>
       <c r="M18">
-        <v>1.088587579263204</v>
+        <v>1.089147757050916</v>
       </c>
       <c r="N18">
-        <v>0.9269355032269437</v>
+        <v>0.989582636529164</v>
       </c>
       <c r="O18">
-        <v>1.047706556614987</v>
+        <v>1.049209035181111</v>
       </c>
       <c r="P18">
-        <v>1.207720122488238</v>
+        <v>1.198683548120298</v>
       </c>
       <c r="Q18">
-        <v>1.151406130392854</v>
+        <v>1.148071519109561</v>
       </c>
       <c r="R18">
-        <v>1.219519675521085</v>
+        <v>1.272001225765047</v>
       </c>
       <c r="S18">
-        <v>1.103358078668907</v>
+        <v>1.106157764472838</v>
       </c>
     </row>
     <row r="19">
@@ -1576,52 +1576,52 @@
         </is>
       </c>
       <c r="D19">
-        <v>0.1737498268147524</v>
+        <v>0.1723639901618951</v>
       </c>
       <c r="E19">
-        <v>0.7350304372034374</v>
+        <v>0.735607700466184</v>
       </c>
       <c r="F19">
-        <v>0.008929844641825516</v>
+        <v>0.008957292836096182</v>
       </c>
       <c r="G19">
-        <v>0.7712961313750915</v>
+        <v>0.7711854479245123</v>
       </c>
       <c r="H19">
-        <v>1.130363315869883</v>
+        <v>1.128989879925328</v>
       </c>
       <c r="I19">
-        <v>1.101589580515479</v>
+        <v>1.101293498993896</v>
       </c>
       <c r="J19">
-        <v>1.132914905882109</v>
+        <v>1.167772174530223</v>
       </c>
       <c r="K19">
-        <v>1.075807362844742</v>
+        <v>1.077319093124362</v>
       </c>
       <c r="L19">
-        <v>1.052815520546763</v>
+        <v>1.055587566511104</v>
       </c>
       <c r="M19">
-        <v>1.077949976174376</v>
+        <v>1.07693141268715</v>
       </c>
       <c r="N19">
-        <v>1.001960602022187</v>
+        <v>1.04006896587321</v>
       </c>
       <c r="O19">
-        <v>1.051911592115921</v>
+        <v>1.054806646306896</v>
       </c>
       <c r="P19">
-        <v>1.216269105300662</v>
+        <v>1.210008287976656</v>
       </c>
       <c r="Q19">
-        <v>1.128794505774226</v>
+        <v>1.125901867150713</v>
       </c>
       <c r="R19">
-        <v>1.270580219275513</v>
+        <v>1.316929734957087</v>
       </c>
       <c r="S19">
-        <v>1.102033319354732</v>
+        <v>1.101513263899547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>